<commit_message>
Lead time + small bug
- implement lead time (works)
- bug in cheapest product calculation
- To do: DEBUG VSS calculation
</commit_message>
<xml_diff>
--- a/Data/capacities_and_investments.xlsx
+++ b/Data/capacities_and_investments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\egbertrv\Documents\GitHub\AIM_Norwegian_Freight_Model\Data\Reorganized\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5084B181-8803-4E25-8784-F2E746FB538F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{5084B181-8803-4E25-8784-F2E746FB538F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D04917C2-918E-4517-92D4-5D8B4E825D37}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13785" windowHeight="23400" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cap rail" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="64">
   <si>
     <t>Bane</t>
   </si>
@@ -217,6 +217,21 @@
   <si>
     <t>Biogas</t>
   </si>
+  <si>
+    <t>Ledetid</t>
+  </si>
+  <si>
+    <t>Leadtime</t>
+  </si>
+  <si>
+    <t>LeadtimeCombi</t>
+  </si>
+  <si>
+    <t>LeadtimeTimber</t>
+  </si>
+  <si>
+    <t>UPDATE LEDETID, den er nå ikke avhengig av distansen</t>
+  </si>
 </sst>
 </file>
 
@@ -226,11 +241,18 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@"/>
     <numFmt numFmtId="165" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -385,56 +407,57 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,7 +676,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2059,10 +2082,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:W998"/>
+  <dimension ref="A1:Y998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2090,7 +2113,7 @@
     <col min="24" max="29" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>43</v>
       </c>
@@ -2112,7 +2135,9 @@
       <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="J1" s="36" t="s">
         <v>46</v>
       </c>
@@ -2134,6 +2159,9 @@
       <c r="P1" s="8" t="s">
         <v>50</v>
       </c>
+      <c r="Q1" s="36" t="s">
+        <v>60</v>
+      </c>
       <c r="S1" s="2" t="s">
         <v>15</v>
       </c>
@@ -2149,8 +2177,14 @@
       <c r="W1" s="8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2173,7 +2207,9 @@
         <f>G14</f>
         <v>226666666.66666666</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="4">
+        <v>5</v>
+      </c>
       <c r="J2" s="40" t="s">
         <v>29</v>
       </c>
@@ -2195,6 +2231,9 @@
       <c r="P2" s="12">
         <v>3300000000</v>
       </c>
+      <c r="Q2" s="43">
+        <v>5</v>
+      </c>
       <c r="S2" s="34" t="s">
         <v>28</v>
       </c>
@@ -2210,8 +2249,14 @@
       <c r="W2" s="4">
         <v>120000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X2" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2234,7 +2279,9 @@
         <f>G14</f>
         <v>226666666.66666666</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="4">
+        <v>5</v>
+      </c>
       <c r="J3" s="38" t="s">
         <v>29</v>
       </c>
@@ -2258,6 +2305,9 @@
         <f>1500000000+375000000</f>
         <v>1875000000</v>
       </c>
+      <c r="Q3">
+        <v>5</v>
+      </c>
       <c r="S3" s="34" t="s">
         <v>31</v>
       </c>
@@ -2273,8 +2323,14 @@
       <c r="W3" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X3" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y3" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2296,7 +2352,9 @@
       <c r="G4" s="4">
         <v>289000000</v>
       </c>
-      <c r="H4" s="4"/>
+      <c r="H4" s="4">
+        <v>5</v>
+      </c>
       <c r="J4" s="35" t="s">
         <v>30</v>
       </c>
@@ -2318,6 +2376,9 @@
       <c r="P4" s="12">
         <v>500000000</v>
       </c>
+      <c r="Q4" s="43">
+        <v>5</v>
+      </c>
       <c r="S4" s="34" t="s">
         <v>35</v>
       </c>
@@ -2333,8 +2394,14 @@
       <c r="W4" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X4" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2356,7 +2423,9 @@
       <c r="G5" s="4">
         <v>275000000</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="4">
+        <v>5</v>
+      </c>
       <c r="S5" s="34" t="s">
         <v>32</v>
       </c>
@@ -2372,8 +2441,14 @@
       <c r="W5" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X5" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2395,7 +2470,9 @@
       <c r="G6" s="9">
         <v>100000000</v>
       </c>
-      <c r="H6" s="9"/>
+      <c r="H6" s="9">
+        <v>5</v>
+      </c>
       <c r="S6" s="34" t="s">
         <v>33</v>
       </c>
@@ -2411,8 +2488,14 @@
       <c r="W6" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X6" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y6" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2434,7 +2517,9 @@
       <c r="G7" s="4">
         <v>275000000</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7" s="4">
+        <v>5</v>
+      </c>
       <c r="S7" s="34" t="s">
         <v>29</v>
       </c>
@@ -2450,8 +2535,14 @@
       <c r="W7" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X7" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2473,7 +2564,9 @@
       <c r="G8" s="4">
         <v>430000000</v>
       </c>
-      <c r="H8" s="4"/>
+      <c r="H8" s="4">
+        <v>5</v>
+      </c>
       <c r="S8" s="34" t="s">
         <v>34</v>
       </c>
@@ -2489,8 +2582,14 @@
       <c r="W8" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X8" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y8" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2512,7 +2611,9 @@
       <c r="G9" s="10">
         <v>500000000</v>
       </c>
-      <c r="H9" s="10"/>
+      <c r="H9" s="4">
+        <v>5</v>
+      </c>
       <c r="S9" s="34" t="s">
         <v>30</v>
       </c>
@@ -2528,8 +2629,14 @@
       <c r="W9" s="4">
         <v>300000000</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X9" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y9" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2551,7 +2658,9 @@
       <c r="G10" s="4">
         <v>927000000</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="4">
+        <v>5</v>
+      </c>
       <c r="S10" s="34" t="s">
         <v>41</v>
       </c>
@@ -2567,8 +2676,14 @@
       <c r="W10" s="4">
         <v>30000000</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X10" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y10" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2590,7 +2705,9 @@
       <c r="G11" s="9">
         <v>100000000</v>
       </c>
-      <c r="H11" s="9"/>
+      <c r="H11" s="4">
+        <v>5</v>
+      </c>
       <c r="S11" s="34" t="s">
         <v>36</v>
       </c>
@@ -2606,8 +2723,14 @@
       <c r="W11" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X11" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y11" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2629,9 +2752,11 @@
       <c r="G12" s="4">
         <v>927000000</v>
       </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2653,9 +2778,11 @@
       <c r="G13" s="4">
         <v>113000000000</v>
       </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2678,9 +2805,11 @@
         <f>680000000/3</f>
         <v>226666666.66666666</v>
       </c>
-      <c r="H14" s="19"/>
-    </row>
-    <row r="15" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2702,9 +2831,11 @@
       <c r="G15" s="19">
         <v>0</v>
       </c>
-      <c r="H15" s="19"/>
-    </row>
-    <row r="16" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="H15" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
@@ -4889,7 +5020,7 @@
   <dimension ref="B1:K997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4923,6 +5054,9 @@
       <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="F1" s="36" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="2" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="32" t="s">
@@ -4937,6 +5071,9 @@
       <c r="E2">
         <v>523021000</v>
       </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
       <c r="G2" s="19"/>
       <c r="K2" s="19"/>
     </row>
@@ -4953,6 +5090,9 @@
       <c r="E3">
         <v>1030229000</v>
       </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="32" t="s">
@@ -4967,6 +5107,9 @@
       <c r="E4">
         <v>260408000</v>
       </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="32" t="s">
@@ -4981,6 +5124,9 @@
       <c r="E5">
         <v>614315000</v>
       </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="32" t="s">
@@ -4995,6 +5141,9 @@
       <c r="E6">
         <v>2685461000</v>
       </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="32" t="s">
@@ -5009,6 +5158,9 @@
       <c r="E7">
         <v>491148000</v>
       </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="32" t="s">
@@ -5023,6 +5175,9 @@
       <c r="E8">
         <v>209400000</v>
       </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="32" t="s">
@@ -5037,6 +5192,9 @@
       <c r="E9">
         <v>1416610000</v>
       </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="32" t="s">
@@ -5050,6 +5208,9 @@
       </c>
       <c r="E10">
         <v>255092000</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
       </c>
       <c r="G10" s="25"/>
       <c r="K10" s="25"/>
@@ -6049,10 +6210,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5788103D-4203-4CBA-AFEE-D82DB11621B2}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6063,7 +6224,7 @@
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>44</v>
       </c>
@@ -6079,8 +6240,11 @@
       <c r="E1" s="42" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>55</v>
       </c>
@@ -6096,8 +6260,14 @@
       <c r="E2" s="42">
         <v>40000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>55</v>
       </c>
@@ -6113,8 +6283,11 @@
       <c r="E3" s="42">
         <v>2500000</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
         <v>55</v>
       </c>
@@ -6129,6 +6302,9 @@
       </c>
       <c r="E4" s="42">
         <v>20000000</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First step in adding extra edges
</commit_message>
<xml_diff>
--- a/Data/capacities_and_investments.xlsx
+++ b/Data/capacities_and_investments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{5084B181-8803-4E25-8784-F2E746FB538F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D04917C2-918E-4517-92D4-5D8B4E825D37}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="13_ncr:1_{5084B181-8803-4E25-8784-F2E746FB538F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE4B6C97-67D6-47AA-8F65-303331111FBB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13785" windowHeight="23400" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13800" yWindow="0" windowWidth="22710" windowHeight="23400" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cap rail" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="74">
   <si>
     <t>Bane</t>
   </si>
@@ -231,6 +231,36 @@
   </si>
   <si>
     <t>UPDATE LEDETID, den er nå ikke avhengig av distansen</t>
+  </si>
+  <si>
+    <t>Europa</t>
+  </si>
+  <si>
+    <t>DETTE BURDE VÆRE NARVIK -&gt; UPDATE</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>no boundaries on terminal capacity</t>
+  </si>
+  <si>
+    <t>UPDATE!</t>
+  </si>
+  <si>
+    <t>burde gå til Narvik</t>
+  </si>
+  <si>
+    <t>introduce extra node in middle</t>
+  </si>
+  <si>
+    <t>Meråkerbanen2</t>
+  </si>
+  <si>
+    <t>ToNarvik</t>
+  </si>
+  <si>
+    <t>EuropaBanen</t>
   </si>
 </sst>
 </file>
@@ -241,11 +271,18 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@"/>
     <numFmt numFmtId="165" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -386,6 +423,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -407,57 +450,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,6 +518,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -673,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -686,15 +735,15 @@
     <col min="3" max="3" width="26.5703125" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="26" width="8.7109375" customWidth="1"/>
+    <col min="6" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="27" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
         <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -709,403 +758,516 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>41</v>
       </c>
       <c r="E2" s="4">
         <v>1250000</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="H2" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="4">
+      <c r="I2" s="4">
         <v>6365000</v>
       </c>
-      <c r="I2" s="4">
+      <c r="J2" s="4">
         <v>380000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>35</v>
       </c>
       <c r="E3" s="4">
         <v>1250000</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="H3" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="4">
+      <c r="I3" s="4">
         <v>475000</v>
       </c>
-      <c r="I3" s="7">
+      <c r="J3" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>32</v>
       </c>
       <c r="E4" s="4">
         <v>1500000</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="H4" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="4">
+      <c r="I4" s="4">
         <v>1425000</v>
       </c>
-      <c r="I4" s="7">
+      <c r="J4" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="4">
         <v>1600000</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="4">
+      <c r="I5" s="4">
         <v>1377500</v>
       </c>
-      <c r="I5" s="7">
+      <c r="J5" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="4">
         <v>250000</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="4">
+      <c r="I6" s="4">
         <v>285000</v>
       </c>
-      <c r="I6" s="7">
+      <c r="J6" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="4">
         <v>1600000</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="4">
+      <c r="I7" s="4">
         <v>1330000</v>
       </c>
-      <c r="I7" s="7">
+      <c r="J7" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>34</v>
       </c>
       <c r="E8" s="4">
         <v>650000</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="4">
+      <c r="I8" s="4">
         <v>1780300</v>
       </c>
-      <c r="I8" s="7">
+      <c r="J8" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="4">
         <v>1000000</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="H9" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="7">
+      <c r="I9" s="6">
         <v>0</v>
       </c>
-      <c r="I9" s="4">
+      <c r="J9" s="4">
         <v>1785000</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="4">
         <v>800000</v>
       </c>
-      <c r="G10" s="26" t="s">
+      <c r="H10" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="7">
+      <c r="I10" s="6">
         <v>0</v>
       </c>
-      <c r="I10" s="4">
+      <c r="J10" s="4">
         <v>56000</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="23" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="4">
         <v>250000</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="H11" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="7">
+      <c r="I11" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="J11" s="13">
         <v>0</v>
       </c>
-      <c r="I11" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="23" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="4">
         <v>950000</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="4">
+        <v>5000000</v>
+      </c>
+      <c r="J12" s="13">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="4">
+        <v>5000000</v>
+      </c>
+      <c r="J13" s="13">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="22" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="4">
         <v>1250000</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="4">
+        <v>5000000</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>66</v>
+      </c>
+      <c r="M14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="19">
         <v>250000</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="6"/>
-    </row>
-    <row r="17" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="4"/>
+      <c r="J15" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="19">
+        <v>250000</v>
+      </c>
+      <c r="F16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="4">
+        <v>950000</v>
+      </c>
+      <c r="F17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="4">
+        <v>2000000</v>
+      </c>
+      <c r="F18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
-      <c r="D23" s="7"/>
-    </row>
-    <row r="24" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
-      <c r="C26" s="7"/>
+      <c r="C26" s="6"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
-      <c r="C27" s="7"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2084,8 +2246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y998"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2114,7 +2276,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -2129,7 +2291,7 @@
       <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -2138,7 +2300,7 @@
       <c r="H1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>46</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -2153,34 +2315,34 @@
       <c r="N1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>60</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2191,10 +2353,10 @@
       <c r="B2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="31" t="s">
         <v>41</v>
       </c>
       <c r="E2" s="4">
@@ -2208,33 +2370,33 @@
         <v>226666666.66666666</v>
       </c>
       <c r="H2" s="4">
-        <v>5</v>
-      </c>
-      <c r="J2" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="K2" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="37">
+      <c r="M2" s="36">
         <v>1</v>
       </c>
       <c r="N2" s="3">
         <v>729</v>
       </c>
-      <c r="O2" s="12">
+      <c r="O2" s="11">
         <v>14000000000</v>
       </c>
-      <c r="P2" s="12">
+      <c r="P2" s="11">
         <v>3300000000</v>
       </c>
-      <c r="Q2" s="43">
-        <v>5</v>
-      </c>
-      <c r="S2" s="34" t="s">
+      <c r="Q2" s="42">
+        <v>6</v>
+      </c>
+      <c r="S2" s="33" t="s">
         <v>28</v>
       </c>
       <c r="T2" s="4">
@@ -2249,10 +2411,10 @@
       <c r="W2" s="4">
         <v>120000000</v>
       </c>
-      <c r="X2" s="25">
+      <c r="X2" s="24">
         <v>3</v>
       </c>
-      <c r="Y2" s="25">
+      <c r="Y2" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2263,10 +2425,10 @@
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>35</v>
       </c>
       <c r="E3" s="4">
@@ -2280,35 +2442,35 @@
         <v>226666666.66666666</v>
       </c>
       <c r="H3" s="4">
-        <v>5</v>
-      </c>
-      <c r="J3" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="39" t="s">
+      <c r="K3" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="37" t="s">
+      <c r="L3" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="M3" s="37">
+      <c r="M3" s="36">
         <v>2</v>
       </c>
       <c r="N3" s="3">
         <v>382</v>
       </c>
-      <c r="O3" s="22">
+      <c r="O3" s="21">
         <f>6500000000+1600000000</f>
         <v>8100000000</v>
       </c>
-      <c r="P3" s="12">
+      <c r="P3" s="11">
         <f>1500000000+375000000</f>
         <v>1875000000</v>
       </c>
       <c r="Q3">
-        <v>5</v>
-      </c>
-      <c r="S3" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" s="33" t="s">
         <v>31</v>
       </c>
       <c r="T3" s="4">
@@ -2317,16 +2479,16 @@
       <c r="U3" s="4">
         <v>210600000</v>
       </c>
-      <c r="V3" s="13">
+      <c r="V3" s="12">
         <v>0</v>
       </c>
-      <c r="W3" s="13">
+      <c r="W3" s="12">
         <v>0</v>
       </c>
-      <c r="X3" s="25">
+      <c r="X3" s="24">
         <v>3</v>
       </c>
-      <c r="Y3" s="25">
+      <c r="Y3" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2337,10 +2499,10 @@
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="31" t="s">
         <v>32</v>
       </c>
       <c r="E4" s="4">
@@ -2353,33 +2515,33 @@
         <v>289000000</v>
       </c>
       <c r="H4" s="4">
-        <v>5</v>
-      </c>
-      <c r="J4" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="37" t="s">
+      <c r="L4" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="37">
+      <c r="M4" s="36">
         <v>1</v>
       </c>
       <c r="N4" s="3">
         <v>115</v>
       </c>
-      <c r="O4" s="12">
+      <c r="O4" s="11">
         <v>2200000000</v>
       </c>
-      <c r="P4" s="12">
+      <c r="P4" s="11">
         <v>500000000</v>
       </c>
-      <c r="Q4" s="43">
-        <v>5</v>
-      </c>
-      <c r="S4" s="34" t="s">
+      <c r="Q4" s="42">
+        <v>6</v>
+      </c>
+      <c r="S4" s="33" t="s">
         <v>35</v>
       </c>
       <c r="T4" s="4">
@@ -2388,16 +2550,16 @@
       <c r="U4" s="4">
         <v>526500000</v>
       </c>
-      <c r="V4" s="13">
+      <c r="V4" s="12">
         <v>0</v>
       </c>
-      <c r="W4" s="13">
+      <c r="W4" s="12">
         <v>0</v>
       </c>
-      <c r="X4" s="25">
+      <c r="X4" s="24">
         <v>3</v>
       </c>
-      <c r="Y4" s="25">
+      <c r="Y4" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2408,10 +2570,10 @@
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="31" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="4">
@@ -2424,9 +2586,9 @@
         <v>275000000</v>
       </c>
       <c r="H5" s="4">
-        <v>5</v>
-      </c>
-      <c r="S5" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="S5" s="33" t="s">
         <v>32</v>
       </c>
       <c r="T5" s="4">
@@ -2435,16 +2597,16 @@
       <c r="U5" s="4">
         <v>526500000</v>
       </c>
-      <c r="V5" s="13">
+      <c r="V5" s="12">
         <v>0</v>
       </c>
-      <c r="W5" s="13">
+      <c r="W5" s="12">
         <v>0</v>
       </c>
-      <c r="X5" s="25">
+      <c r="X5" s="24">
         <v>3</v>
       </c>
-      <c r="Y5" s="25">
+      <c r="Y5" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2455,25 +2617,25 @@
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="31" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="4">
         <v>250000</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>500000</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>100000000</v>
       </c>
-      <c r="H6" s="9">
-        <v>5</v>
-      </c>
-      <c r="S6" s="34" t="s">
+      <c r="H6" s="4">
+        <v>8</v>
+      </c>
+      <c r="S6" s="33" t="s">
         <v>33</v>
       </c>
       <c r="T6" s="4">
@@ -2482,16 +2644,16 @@
       <c r="U6" s="4">
         <v>210600000</v>
       </c>
-      <c r="V6" s="13">
+      <c r="V6" s="12">
         <v>0</v>
       </c>
-      <c r="W6" s="13">
+      <c r="W6" s="12">
         <v>0</v>
       </c>
-      <c r="X6" s="25">
+      <c r="X6" s="24">
         <v>3</v>
       </c>
-      <c r="Y6" s="25">
+      <c r="Y6" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2499,13 +2661,13 @@
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="31" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="4">
@@ -2518,9 +2680,9 @@
         <v>275000000</v>
       </c>
       <c r="H7" s="4">
-        <v>5</v>
-      </c>
-      <c r="S7" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="S7" s="33" t="s">
         <v>29</v>
       </c>
       <c r="T7" s="4">
@@ -2529,16 +2691,16 @@
       <c r="U7" s="4">
         <v>526500000</v>
       </c>
-      <c r="V7" s="13">
+      <c r="V7" s="12">
         <v>0</v>
       </c>
-      <c r="W7" s="13">
+      <c r="W7" s="12">
         <v>0</v>
       </c>
-      <c r="X7" s="25">
+      <c r="X7" s="24">
         <v>3</v>
       </c>
-      <c r="Y7" s="25">
+      <c r="Y7" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2549,10 +2711,10 @@
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="31" t="s">
         <v>34</v>
       </c>
       <c r="E8" s="4">
@@ -2565,9 +2727,9 @@
         <v>430000000</v>
       </c>
       <c r="H8" s="4">
-        <v>5</v>
-      </c>
-      <c r="S8" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="S8" s="33" t="s">
         <v>34</v>
       </c>
       <c r="T8" s="4">
@@ -2576,16 +2738,16 @@
       <c r="U8" s="4">
         <v>526500000</v>
       </c>
-      <c r="V8" s="13">
+      <c r="V8" s="12">
         <v>0</v>
       </c>
-      <c r="W8" s="13">
+      <c r="W8" s="12">
         <v>0</v>
       </c>
-      <c r="X8" s="25">
+      <c r="X8" s="24">
         <v>3</v>
       </c>
-      <c r="Y8" s="25">
+      <c r="Y8" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2596,10 +2758,10 @@
       <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="31" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="4">
@@ -2608,13 +2770,13 @@
       <c r="F9" s="4">
         <v>1500000</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>500000000</v>
       </c>
       <c r="H9" s="4">
-        <v>5</v>
-      </c>
-      <c r="S9" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="S9" s="33" t="s">
         <v>30</v>
       </c>
       <c r="T9" s="4">
@@ -2629,10 +2791,10 @@
       <c r="W9" s="4">
         <v>300000000</v>
       </c>
-      <c r="X9" s="25">
+      <c r="X9" s="24">
         <v>3</v>
       </c>
-      <c r="Y9" s="25">
+      <c r="Y9" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2643,10 +2805,10 @@
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="31" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="4">
@@ -2659,9 +2821,9 @@
         <v>927000000</v>
       </c>
       <c r="H10" s="4">
-        <v>5</v>
-      </c>
-      <c r="S10" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="S10" s="33" t="s">
         <v>41</v>
       </c>
       <c r="T10" s="4">
@@ -2676,10 +2838,10 @@
       <c r="W10" s="4">
         <v>30000000</v>
       </c>
-      <c r="X10" s="25">
+      <c r="X10" s="24">
         <v>3</v>
       </c>
-      <c r="Y10" s="25">
+      <c r="Y10" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2690,25 +2852,25 @@
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="31" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="4">
         <v>250000</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>500000</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>100000000</v>
       </c>
       <c r="H11" s="4">
-        <v>5</v>
-      </c>
-      <c r="S11" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="S11" s="33" t="s">
         <v>36</v>
       </c>
       <c r="T11" s="4">
@@ -2717,16 +2879,16 @@
       <c r="U11" s="4">
         <v>210600000</v>
       </c>
-      <c r="V11" s="13">
+      <c r="V11" s="12">
         <v>0</v>
       </c>
-      <c r="W11" s="13">
+      <c r="W11" s="12">
         <v>0</v>
       </c>
-      <c r="X11" s="25">
+      <c r="X11" s="24">
         <v>3</v>
       </c>
-      <c r="Y11" s="25">
+      <c r="Y11" s="24">
         <v>3</v>
       </c>
     </row>
@@ -2737,10 +2899,10 @@
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="31" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="4">
@@ -2753,20 +2915,20 @@
         <v>927000000</v>
       </c>
       <c r="H12" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="31" t="s">
         <v>36</v>
       </c>
       <c r="E13" s="4">
@@ -2789,50 +2951,50 @@
       <c r="B14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="19">
         <v>150000</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="19">
         <v>1400000</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="18">
         <f>680000000/3</f>
         <v>226666666.66666666</v>
       </c>
       <c r="H14" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="19">
         <v>0</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="19">
         <v>250000</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="18">
         <v>0</v>
       </c>
       <c r="H15" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2841,39 +3003,39 @@
       <c r="B18" s="1"/>
     </row>
     <row r="19" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
+      <c r="B19" s="10"/>
     </row>
     <row r="20" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="J21" s="12"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="J21" s="11"/>
     </row>
     <row r="22" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="12"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="11"/>
     </row>
     <row r="23" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
     </row>
     <row r="24" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="12"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2885,10 +3047,10 @@
     <row r="30" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
     </row>
     <row r="32" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
@@ -2901,43 +3063,43 @@
       <c r="B33" s="3"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
     </row>
     <row r="34" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
     </row>
     <row r="35" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
     </row>
     <row r="36" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
     </row>
     <row r="37" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="3"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
     </row>
     <row r="38" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
     </row>
     <row r="39" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
@@ -2957,8 +3119,8 @@
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
     </row>
     <row r="42" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3928,7 +4090,7 @@
   <dimension ref="B1:E997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C2:C10"/>
+      <selection activeCell="B2" sqref="B2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3950,75 +4112,75 @@
       </c>
     </row>
     <row r="2" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="28">
         <v>19498000</v>
       </c>
-      <c r="E2" s="19"/>
+      <c r="E2" s="18"/>
     </row>
     <row r="3" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="28">
         <v>38407000</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="28">
         <v>9708000</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="28">
         <v>22902000</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="28">
         <v>100114000</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="28">
         <v>18310000</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="28">
         <v>7806000</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="28">
         <v>52811000</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="28">
         <v>9510000</v>
       </c>
     </row>
@@ -5054,12 +5216,12 @@
       <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>28</v>
       </c>
       <c r="C2">
@@ -5074,11 +5236,11 @@
       <c r="F2">
         <v>3</v>
       </c>
-      <c r="G2" s="19"/>
-      <c r="K2" s="19"/>
+      <c r="G2" s="18"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>41</v>
       </c>
       <c r="C3">
@@ -5095,7 +5257,7 @@
       </c>
     </row>
     <row r="4" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C4">
@@ -5112,7 +5274,7 @@
       </c>
     </row>
     <row r="5" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="31" t="s">
         <v>35</v>
       </c>
       <c r="C5">
@@ -5129,7 +5291,7 @@
       </c>
     </row>
     <row r="6" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="31" t="s">
         <v>32</v>
       </c>
       <c r="C6">
@@ -5146,7 +5308,7 @@
       </c>
     </row>
     <row r="7" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
         <v>33</v>
       </c>
       <c r="C7">
@@ -5163,7 +5325,7 @@
       </c>
     </row>
     <row r="8" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="31" t="s">
         <v>29</v>
       </c>
       <c r="C8">
@@ -5180,7 +5342,7 @@
       </c>
     </row>
     <row r="9" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="31" t="s">
         <v>34</v>
       </c>
       <c r="C9">
@@ -5197,7 +5359,7 @@
       </c>
     </row>
     <row r="10" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="31" t="s">
         <v>36</v>
       </c>
       <c r="C10">
@@ -5212,8 +5374,8 @@
       <c r="F10">
         <v>3</v>
       </c>
-      <c r="G10" s="25"/>
-      <c r="K10" s="25"/>
+      <c r="G10" s="24"/>
+      <c r="K10" s="24"/>
     </row>
     <row r="11" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6213,7 +6375,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6225,19 +6387,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="41" t="s">
         <v>54</v>
       </c>
       <c r="F1" t="s">
@@ -6245,19 +6407,19 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="42">
+      <c r="C2" s="41">
         <v>150</v>
       </c>
-      <c r="D2" s="42">
+      <c r="D2" s="41">
         <v>360</v>
       </c>
-      <c r="E2" s="42">
+      <c r="E2" s="41">
         <v>40000000</v>
       </c>
       <c r="F2">
@@ -6268,19 +6430,19 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3" s="41">
         <v>100</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="41">
         <v>10</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="41">
         <v>2500000</v>
       </c>
       <c r="F3">
@@ -6288,19 +6450,19 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="41">
         <v>300</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="41">
         <v>180</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="41">
         <v>20000000</v>
       </c>
       <c r="F4">

</xml_diff>

<commit_message>
Bug investments + updated lead times
</commit_message>
<xml_diff>
--- a/Data/capacities_and_investments.xlsx
+++ b/Data/capacities_and_investments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="13_ncr:1_{5084B181-8803-4E25-8784-F2E746FB538F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE4B6C97-67D6-47AA-8F65-303331111FBB}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="13_ncr:1_{5084B181-8803-4E25-8784-F2E746FB538F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F913E53B-EB0B-4412-9B10-7E3D53B57437}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="0" windowWidth="22710" windowHeight="23400" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13800" yWindow="0" windowWidth="30345" windowHeight="23400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cap rail" sheetId="1" r:id="rId1"/>
@@ -230,9 +230,6 @@
     <t>LeadtimeTimber</t>
   </si>
   <si>
-    <t>UPDATE LEDETID, den er nå ikke avhengig av distansen</t>
-  </si>
-  <si>
     <t>Europa</t>
   </si>
   <si>
@@ -261,6 +258,9 @@
   </si>
   <si>
     <t>EuropaBanen</t>
+  </si>
+  <si>
+    <t>UPDATE LEDETID, den er nå ikke avhengig av distansen, elns</t>
   </si>
 </sst>
 </file>
@@ -520,10 +520,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -1028,7 +1024,7 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1057,10 +1053,10 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
+        <v>65</v>
+      </c>
+      <c r="M12" t="s">
         <v>66</v>
-      </c>
-      <c r="M12" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1089,10 +1085,10 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
+        <v>65</v>
+      </c>
+      <c r="M13" t="s">
         <v>66</v>
-      </c>
-      <c r="M13" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1112,7 +1108,7 @@
         <v>1250000</v>
       </c>
       <c r="H14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I14" s="4">
         <v>5000000</v>
@@ -1121,10 +1117,10 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
+        <v>65</v>
+      </c>
+      <c r="M14" t="s">
         <v>66</v>
-      </c>
-      <c r="M14" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1153,7 +1149,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" s="23" t="s">
         <v>29</v>
@@ -1165,10 +1161,10 @@
         <v>250000</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="13">
@@ -1180,7 +1176,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" s="23" t="s">
         <v>13</v>
@@ -1192,10 +1188,10 @@
         <v>950000</v>
       </c>
       <c r="F17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" t="s">
         <v>68</v>
-      </c>
-      <c r="G17" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1203,19 +1199,19 @@
         <v>1</v>
       </c>
       <c r="B18" s="45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="23" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E18" s="4">
         <v>2000000</v>
       </c>
       <c r="F18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2246,8 +2242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2370,7 +2366,7 @@
         <v>226666666.66666666</v>
       </c>
       <c r="H2" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J2" s="39" t="s">
         <v>29</v>
@@ -2412,10 +2408,10 @@
         <v>120000000</v>
       </c>
       <c r="X2" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y2" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2442,7 +2438,7 @@
         <v>226666666.66666666</v>
       </c>
       <c r="H3" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J3" s="37" t="s">
         <v>29</v>
@@ -2486,10 +2482,10 @@
         <v>0</v>
       </c>
       <c r="X3" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y3" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2515,7 +2511,7 @@
         <v>289000000</v>
       </c>
       <c r="H4" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J4" s="34" t="s">
         <v>30</v>
@@ -2557,10 +2553,10 @@
         <v>0</v>
       </c>
       <c r="X4" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y4" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2586,7 +2582,7 @@
         <v>275000000</v>
       </c>
       <c r="H5" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="S5" s="33" t="s">
         <v>32</v>
@@ -2604,10 +2600,10 @@
         <v>0</v>
       </c>
       <c r="X5" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y5" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2633,7 +2629,7 @@
         <v>100000000</v>
       </c>
       <c r="H6" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="S6" s="33" t="s">
         <v>33</v>
@@ -2651,10 +2647,10 @@
         <v>0</v>
       </c>
       <c r="X6" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y6" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2680,7 +2676,7 @@
         <v>275000000</v>
       </c>
       <c r="H7" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="S7" s="33" t="s">
         <v>29</v>
@@ -2698,10 +2694,10 @@
         <v>0</v>
       </c>
       <c r="X7" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y7" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2727,7 +2723,7 @@
         <v>430000000</v>
       </c>
       <c r="H8" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="S8" s="33" t="s">
         <v>34</v>
@@ -2745,10 +2741,10 @@
         <v>0</v>
       </c>
       <c r="X8" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y8" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2774,7 +2770,7 @@
         <v>500000000</v>
       </c>
       <c r="H9" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="S9" s="33" t="s">
         <v>30</v>
@@ -2792,10 +2788,10 @@
         <v>300000000</v>
       </c>
       <c r="X9" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y9" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2821,7 +2817,7 @@
         <v>927000000</v>
       </c>
       <c r="H10" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="S10" s="33" t="s">
         <v>41</v>
@@ -2839,10 +2835,10 @@
         <v>30000000</v>
       </c>
       <c r="X10" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y10" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2868,7 +2864,7 @@
         <v>100000000</v>
       </c>
       <c r="H11" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="S11" s="33" t="s">
         <v>36</v>
@@ -2886,10 +2882,10 @@
         <v>0</v>
       </c>
       <c r="X11" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y11" s="24">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2915,7 +2911,7 @@
         <v>927000000</v>
       </c>
       <c r="H12" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2941,7 +2937,7 @@
         <v>113000000000</v>
       </c>
       <c r="H13" s="4">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2968,7 +2964,7 @@
         <v>226666666.66666666</v>
       </c>
       <c r="H14" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2994,7 +2990,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4090,7 +4086,7 @@
   <dimension ref="B1:E997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B10"/>
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5182,7 +5178,7 @@
   <dimension ref="B1:K997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="F2" sqref="F2:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5234,7 +5230,7 @@
         <v>523021000</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G2" s="18"/>
       <c r="K2" s="18"/>
@@ -5253,7 +5249,7 @@
         <v>1030229000</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5270,7 +5266,7 @@
         <v>260408000</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5287,7 +5283,7 @@
         <v>614315000</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5304,7 +5300,7 @@
         <v>2685461000</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5321,7 +5317,7 @@
         <v>491148000</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5338,7 +5334,7 @@
         <v>209400000</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5355,7 +5351,7 @@
         <v>1416610000</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5372,7 +5368,7 @@
         <v>255092000</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G10" s="24"/>
       <c r="K10" s="24"/>
@@ -6374,8 +6370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5788103D-4203-4CBA-AFEE-D82DB11621B2}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6423,10 +6419,10 @@
         <v>40000000</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6446,7 +6442,7 @@
         <v>2500000</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -6466,7 +6462,7 @@
         <v>20000000</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some debug and prepare cluster
</commit_message>
<xml_diff>
--- a/Data/capacities_and_investments.xlsx
+++ b/Data/capacities_and_investments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="13_ncr:1_{5084B181-8803-4E25-8784-F2E746FB538F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6F78F8E-6067-450B-A363-7D0DAA7A8610}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{B0F08328-661E-442A-80EA-83F08B1D30D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13800" yWindow="0" windowWidth="30345" windowHeight="23400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,16 +21,6 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mgsZk5PiUtOKDBIY/SuWxB5nEitHw=="/>
     </ext>
@@ -2246,7 +2236,7 @@
   <dimension ref="A1:AA998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3000,7 +2990,7 @@
         <v>56500000000</v>
       </c>
       <c r="H13" s="4">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I13" s="4">
         <v>113000000000</v>
@@ -6543,4 +6533,300 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085DB58C8134B304E8722528DF46508C9" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6ab0102ed29085baca82ec1af27f0672">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1d2ad661-40b4-4211-810e-9f8311f21e61" xmlns:ns4="e3bebc04-41cd-4c9b-8948-0bf19cce4780" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a32578e7ce5d36f6e724f25bbda53d39" ns3:_="" ns4:_="">
+    <xsd:import namespace="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
+    <xsd:import namespace="e3bebc04-41cd-4c9b-8948-0bf19cce4780"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1d2ad661-40b4-4211-810e-9f8311f21e61" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="MediaServiceAutoTags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="12" nillable="true" ma:displayName="MediaServiceLocation" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="16" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="17" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="21" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_activity" ma:index="22" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e3bebc04-41cd-4c9b-8948-0bf19cce4780" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="20" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1d2ad661-40b4-4211-810e-9f8311f21e61" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79DA533C-9A6E-4D83-BCFC-25254FE6FDCB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
+    <ds:schemaRef ds:uri="e3bebc04-41cd-4c9b-8948-0bf19cce4780"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153AE8AE-6581-44C9-9194-962A53477112}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1F09BEA-AF68-4060-8C78-FF3F1F123D80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="e3bebc04-41cd-4c9b-8948-0bf19cce4780"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed bugs related to capacity data
</commit_message>
<xml_diff>
--- a/Data/capacities_and_investments.xlsx
+++ b/Data/capacities_and_investments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/STraM_ntnu_development/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruben\GitHub\STraM_ntnu_development\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{97909E35-3EF3-4E49-BADC-20215281713F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{712E1ABB-D99C-49B9-B23B-ECC5EED1F17E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F3FDB7-C931-4931-B377-38511D55C441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="28800" windowHeight="22170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="node_capacities" sheetId="9" r:id="rId1"/>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0C314-BCF2-4271-977A-4A8103B5257B}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2151,7 +2151,7 @@
   <dimension ref="A1:S60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P55" sqref="P55"/>
+      <selection activeCell="I52" sqref="I52:J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4216,23 +4216,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1d2ad661-40b4-4211-810e-9f8311f21e61" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085DB58C8134B304E8722528DF46508C9" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6ab0102ed29085baca82ec1af27f0672">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1d2ad661-40b4-4211-810e-9f8311f21e61" xmlns:ns4="e3bebc04-41cd-4c9b-8948-0bf19cce4780" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a32578e7ce5d36f6e724f25bbda53d39" ns3:_="" ns4:_="">
     <xsd:import namespace="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
@@ -4467,10 +4450,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1d2ad661-40b4-4211-810e-9f8311f21e61" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153AE8AE-6581-44C9-9194-962A53477112}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79DA533C-9A6E-4D83-BCFC-25254FE6FDCB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
+    <ds:schemaRef ds:uri="e3bebc04-41cd-4c9b-8948-0bf19cce4780"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4493,20 +4504,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79DA533C-9A6E-4D83-BCFC-25254FE6FDCB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153AE8AE-6581-44C9-9194-962A53477112}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
-    <ds:schemaRef ds:uri="e3bebc04-41cd-4c9b-8948-0bf19cce4780"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
The model runs and produces output/figures
But more debugging remains. Currently, the carbon costs are disproportionally high.

Some of the issues fixed/changes:
- Removed the terminaly capacity issue (maybe due to 0 capacity at NCS)
- Remove the domestic/foreign distinction ("_Norway"). I did not understand why this was necessary in the first place. Capacities can be set in capacities file.
- transfer paths only with transfer in Norway? -> Removed
- Do not leave excel connection open in a class (that was causing some troubles).
</commit_message>
<xml_diff>
--- a/Data/capacities_and_investments.xlsx
+++ b/Data/capacities_and_investments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/STraM_ntnu_development/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{CC5B5A6A-F206-4538-8C7D-60B55F67A255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9521F94-D7AF-4FFC-9201-3276448CD1FF}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{CC5B5A6A-F206-4538-8C7D-60B55F67A255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{437944D0-78E9-48CE-9287-E554586CD4F8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="6590" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="node_capacities" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="83">
   <si>
     <t>Oslo</t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t>Ingen bane!</t>
+  </si>
+  <si>
+    <t>We need to define for sweden as well</t>
+  </si>
+  <si>
+    <t>out of scope, list as infinite capacity</t>
   </si>
 </sst>
 </file>
@@ -721,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0C314-BCF2-4271-977A-4A8103B5257B}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2055,7 +2061,7 @@
       </c>
       <c r="J48" s="16"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>12</v>
       </c>
@@ -2081,7 +2087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>13</v>
       </c>
@@ -2107,7 +2113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>21</v>
       </c>
@@ -2132,8 +2138,11 @@
       <c r="H51" s="23">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>22</v>
       </c>
@@ -2159,7 +2168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>23</v>
       </c>
@@ -2181,8 +2190,11 @@
       <c r="G53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>24</v>
       </c>
@@ -2204,8 +2216,11 @@
       <c r="G54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>25</v>
       </c>
@@ -2219,7 +2234,7 @@
         <v>19</v>
       </c>
       <c r="E55" s="21">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F55" s="23">
         <v>0</v>
@@ -2229,6 +2244,9 @@
       </c>
       <c r="H55" s="23">
         <v>5</v>
+      </c>
+      <c r="I55" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -4326,23 +4344,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1d2ad661-40b4-4211-810e-9f8311f21e61" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085DB58C8134B304E8722528DF46508C9" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80174008b946241598c9c4dc1e838b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1d2ad661-40b4-4211-810e-9f8311f21e61" xmlns:ns4="e3bebc04-41cd-4c9b-8948-0bf19cce4780" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="83c7d99240e58c9b66f78776c092749e" ns3:_="" ns4:_="">
     <xsd:import namespace="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
@@ -4583,32 +4584,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1F09BEA-AF68-4060-8C78-FF3F1F123D80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="e3bebc04-41cd-4c9b-8948-0bf19cce4780"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153AE8AE-6581-44C9-9194-962A53477112}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1d2ad661-40b4-4211-810e-9f8311f21e61" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A60908BF-6965-4963-8A59-4F703B835956}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4625,4 +4618,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153AE8AE-6581-44C9-9194-962A53477112}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1F09BEA-AF68-4060-8C78-FF3F1F123D80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="e3bebc04-41cd-4c9b-8948-0bf19cce4780"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated the calculation of charging infrastructure costs
- The code runs
- DIscussion item: in the visualizations, show charging costs as part of the OPEX, or part of the CAPEX (investments)?
</commit_message>
<xml_diff>
--- a/Data/capacities_and_investments.xlsx
+++ b/Data/capacities_and_investments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/STraM_ntnu_development/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{CC5B5A6A-F206-4538-8C7D-60B55F67A255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEDD09C5-E94C-4632-A4A4-A627B5F6EA34}"/>
+  <xr:revisionPtr revIDLastSave="221" documentId="8_{CC5B5A6A-F206-4538-8C7D-60B55F67A255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4CB2B2C-28F3-4EFE-9BEE-5E14FDC6A945}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="28800" windowHeight="22170" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="node_capacities" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="85">
   <si>
     <t>Oslo</t>
   </si>
@@ -287,7 +287,13 @@
     <t>Station_cost_NOK</t>
   </si>
   <si>
-    <t>Ledetid_year</t>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>we removed the lead time. Only in the first time period we might want to add a hard constraint that captures that it takes some time to create an initial infrastructure</t>
+  </si>
+  <si>
+    <t>the blue values are interpolated</t>
   </si>
 </sst>
 </file>
@@ -442,7 +448,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,6 +458,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -468,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -510,6 +528,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4192,21 +4213,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F55713-1448-49D9-BD60-FDB1E7BDCF91}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>10</v>
       </c>
@@ -4214,59 +4235,322 @@
         <v>58</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="35">
+        <v>2023</v>
+      </c>
+      <c r="D2" s="35">
         <v>150</v>
       </c>
-      <c r="D2">
-        <v>360</v>
-      </c>
-      <c r="E2">
-        <v>40000000</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="H2" s="24" t="s">
+      <c r="E2" s="35">
+        <v>110</v>
+      </c>
+      <c r="F2" s="35">
+        <v>48550</v>
+      </c>
+      <c r="I2" s="24" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="35">
+        <v>2034</v>
+      </c>
+      <c r="D3" s="35">
+        <v>150</v>
+      </c>
+      <c r="E3" s="35">
+        <v>166</v>
+      </c>
+      <c r="F3" s="35">
+        <v>25920</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="35">
+        <v>2050</v>
+      </c>
+      <c r="D4" s="35">
+        <v>150</v>
+      </c>
+      <c r="E4" s="35">
+        <v>166</v>
+      </c>
+      <c r="F4" s="35">
+        <v>25920</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="36">
+        <v>2026</v>
+      </c>
+      <c r="D5" s="36">
+        <v>150</v>
+      </c>
+      <c r="E5" s="37">
+        <f>FORECAST($C5,E$2:E$4,$C$2:$C$4)</f>
+        <v>128.7341772151899</v>
+      </c>
+      <c r="F5" s="37">
+        <f>FORECAST($C5,F$2:F$4,$C$2:$C$4)</f>
+        <v>40979.385171790142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="36">
+        <v>2028</v>
+      </c>
+      <c r="D6" s="36">
+        <v>150</v>
+      </c>
+      <c r="E6" s="37">
+        <f t="shared" ref="E6:F8" si="0">FORECAST($C6,E$2:E$4,$C$2:$C$4)</f>
+        <v>132.58227848101251</v>
+      </c>
+      <c r="F6" s="37">
+        <f t="shared" si="0"/>
+        <v>39424.339963833569</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="36">
+        <v>2030</v>
+      </c>
+      <c r="D7" s="36">
+        <v>150</v>
+      </c>
+      <c r="E7" s="37">
+        <f t="shared" si="0"/>
+        <v>136.43037974683511</v>
+      </c>
+      <c r="F7" s="37">
+        <f t="shared" si="0"/>
+        <v>37869.294755876996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="36">
+        <v>2040</v>
+      </c>
+      <c r="D8" s="36">
+        <v>150</v>
+      </c>
+      <c r="E8" s="37">
+        <f t="shared" si="0"/>
+        <v>155.67088607594906</v>
+      </c>
+      <c r="F8" s="37">
+        <f t="shared" si="0"/>
+        <v>30094.068716093898</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C3">
+      <c r="C9" s="35">
+        <v>2023</v>
+      </c>
+      <c r="D9" s="35">
         <v>100</v>
       </c>
-      <c r="D3">
+      <c r="E9" s="35">
         <v>10</v>
       </c>
-      <c r="E3">
-        <v>2500000</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
+      <c r="F9" s="35">
+        <v>46430</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="35">
+        <v>2034</v>
+      </c>
+      <c r="D10" s="35">
+        <v>100</v>
+      </c>
+      <c r="E10" s="35">
+        <v>20</v>
+      </c>
+      <c r="F10" s="35">
+        <v>42000</v>
+      </c>
+      <c r="I10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="35">
+        <v>2050</v>
+      </c>
+      <c r="D11" s="35">
+        <v>100</v>
+      </c>
+      <c r="E11" s="35">
+        <v>20</v>
+      </c>
+      <c r="F11" s="35">
+        <v>37420</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="36">
+        <v>2026</v>
+      </c>
+      <c r="D12" s="36">
+        <v>100</v>
+      </c>
+      <c r="E12" s="37">
+        <f>FORECAST($C12,E$9:E$11,$C$9:$C$11)</f>
+        <v>13.345388788426703</v>
+      </c>
+      <c r="F12" s="37">
+        <f>FORECAST($C12,F$9:F$11,$C$9:$C$11)</f>
+        <v>45142.622061482864</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="36">
+        <v>2028</v>
+      </c>
+      <c r="D13" s="36">
+        <v>100</v>
+      </c>
+      <c r="E13" s="37">
+        <f t="shared" ref="E13:F15" si="1">FORECAST($C13,E$9:E$11,$C$9:$C$11)</f>
+        <v>14.032549728752201</v>
+      </c>
+      <c r="F13" s="37">
+        <f t="shared" si="1"/>
+        <v>44482.079566003638</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="36">
+        <v>2030</v>
+      </c>
+      <c r="D14" s="36">
+        <v>100</v>
+      </c>
+      <c r="E14" s="37">
+        <f t="shared" si="1"/>
+        <v>14.719710669077699</v>
+      </c>
+      <c r="F14" s="37">
+        <f t="shared" si="1"/>
+        <v>43821.537070524413</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="36">
+        <v>2040</v>
+      </c>
+      <c r="D15" s="36">
+        <v>100</v>
+      </c>
+      <c r="E15" s="37">
+        <f t="shared" si="1"/>
+        <v>18.155515370705189</v>
+      </c>
+      <c r="F15" s="37">
+        <f t="shared" si="1"/>
+        <v>40518.824593128404</v>
       </c>
     </row>
   </sheetData>
@@ -4344,14 +4628,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1d2ad661-40b4-4211-810e-9f8311f21e61" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4360,7 +4636,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085DB58C8134B304E8722528DF46508C9" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80174008b946241598c9c4dc1e838b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1d2ad661-40b4-4211-810e-9f8311f21e61" xmlns:ns4="e3bebc04-41cd-4c9b-8948-0bf19cce4780" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="83c7d99240e58c9b66f78776c092749e" ns3:_="" ns4:_="">
     <xsd:import namespace="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
@@ -4601,24 +4877,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1F09BEA-AF68-4060-8C78-FF3F1F123D80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="e3bebc04-41cd-4c9b-8948-0bf19cce4780"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1d2ad661-40b4-4211-810e-9f8311f21e61" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153AE8AE-6581-44C9-9194-962A53477112}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -4626,7 +4893,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A60908BF-6965-4963-8A59-4F703B835956}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4643,4 +4910,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1F09BEA-AF68-4060-8C78-FF3F1F123D80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="e3bebc04-41cd-4c9b-8948-0bf19cce4780"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
rail cap Sweden, nordnorgebanen
</commit_message>
<xml_diff>
--- a/Data/capacities_and_investments.xlsx
+++ b/Data/capacities_and_investments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/STraM_ntnu_development/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonamar\Documents\04_Papers\Paper IV\Invest_capacity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F7533FD4-2A0E-4671-AE97-CCBF20AF3B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{706DCA58-8010-4862-9022-F66F030C4025}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFE2030-2E27-40C7-BB93-12FB8D99A0E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="28800" windowHeight="22170" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="15996" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="node_capacities" sheetId="9" r:id="rId1"/>
@@ -20,17 +20,6 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataSignature="AMtx7mgsZk5PiUtOKDBIY/SuWxB5nEitHw=="/>
     </ext>
@@ -472,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -503,7 +492,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -729,22 +717,22 @@
       <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>20</v>
       </c>
@@ -775,7 +763,7 @@
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -799,7 +787,7 @@
       </c>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -823,7 +811,7 @@
       </c>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -847,7 +835,7 @@
       </c>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -871,7 +859,7 @@
       </c>
       <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -895,7 +883,7 @@
       </c>
       <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -919,7 +907,7 @@
       </c>
       <c r="I7" s="10"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -943,7 +931,7 @@
       </c>
       <c r="I8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -967,7 +955,7 @@
       </c>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -991,7 +979,7 @@
       </c>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1016,7 +1004,7 @@
       <c r="I11" s="9"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1041,7 +1029,7 @@
       <c r="I12" s="16"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1067,7 +1055,7 @@
       <c r="J13" s="16"/>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1093,7 +1081,7 @@
       <c r="J14" s="16"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>21</v>
       </c>
@@ -1119,7 +1107,7 @@
       <c r="J15" s="16"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>22</v>
       </c>
@@ -1145,7 +1133,7 @@
       <c r="J16" s="16"/>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>23</v>
       </c>
@@ -1171,7 +1159,7 @@
       <c r="J17" s="16"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>24</v>
       </c>
@@ -1197,7 +1185,7 @@
       <c r="J18" s="16"/>
       <c r="K18" s="8"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>25</v>
       </c>
@@ -1223,7 +1211,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="8"/>
     </row>
-    <row r="20" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1257,7 +1245,7 @@
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1290,7 +1278,7 @@
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1322,7 +1310,7 @@
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4</v>
       </c>
@@ -1354,7 +1342,7 @@
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -1386,7 +1374,7 @@
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>6</v>
       </c>
@@ -1417,7 +1405,7 @@
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>7</v>
       </c>
@@ -1449,7 +1437,7 @@
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>8</v>
       </c>
@@ -1481,7 +1469,7 @@
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1513,7 +1501,7 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10</v>
       </c>
@@ -1547,7 +1535,7 @@
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>11</v>
       </c>
@@ -1581,7 +1569,7 @@
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>12</v>
       </c>
@@ -1609,7 +1597,7 @@
       </c>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>13</v>
       </c>
@@ -1635,7 +1623,7 @@
       <c r="I32" s="11"/>
       <c r="K32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>21</v>
       </c>
@@ -1659,7 +1647,7 @@
       </c>
       <c r="K33" s="5"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>22</v>
       </c>
@@ -1683,7 +1671,7 @@
       </c>
       <c r="H34" s="22"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>23</v>
       </c>
@@ -1706,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>24</v>
       </c>
@@ -1729,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>25</v>
       </c>
@@ -1752,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1781,7 +1769,7 @@
       </c>
       <c r="J38" s="11"/>
     </row>
-    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1812,7 +1800,7 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>3</v>
       </c>
@@ -1841,7 +1829,7 @@
       </c>
       <c r="J40" s="12"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1870,7 +1858,7 @@
       </c>
       <c r="J41" s="12"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>5</v>
       </c>
@@ -1899,7 +1887,7 @@
       </c>
       <c r="J42" s="12"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>6</v>
       </c>
@@ -1928,7 +1916,7 @@
       </c>
       <c r="J43" s="12"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>7</v>
       </c>
@@ -1957,7 +1945,7 @@
       </c>
       <c r="J44" s="12"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>8</v>
       </c>
@@ -1983,7 +1971,7 @@
       </c>
       <c r="J45" s="12"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>9</v>
       </c>
@@ -2012,7 +2000,7 @@
       </c>
       <c r="J46" s="12"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10</v>
       </c>
@@ -2041,7 +2029,7 @@
       </c>
       <c r="J47" s="12"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>11</v>
       </c>
@@ -2070,7 +2058,7 @@
       </c>
       <c r="J48" s="12"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>12</v>
       </c>
@@ -2098,7 +2086,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>13</v>
       </c>
@@ -2126,7 +2114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>21</v>
       </c>
@@ -2149,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>22</v>
       </c>
@@ -2172,7 +2160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>23</v>
       </c>
@@ -2195,7 +2183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>24</v>
       </c>
@@ -2218,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>25</v>
       </c>
@@ -2251,31 +2239,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF0D60D-EDFF-4BF0-A9C8-7E20F58C5774}">
   <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>50</v>
       </c>
@@ -2325,7 +2313,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2351,7 +2339,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2377,7 +2365,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2403,7 +2391,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2429,7 +2417,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2455,7 +2443,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2481,7 +2469,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2507,7 +2495,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2533,7 +2521,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2559,7 +2547,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2585,7 +2573,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2611,7 +2599,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2637,7 +2625,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2663,7 +2651,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>22</v>
       </c>
@@ -2689,7 +2677,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>23</v>
       </c>
@@ -2715,7 +2703,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>23</v>
       </c>
@@ -2741,7 +2729,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>8</v>
       </c>
@@ -2767,7 +2755,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>8</v>
       </c>
@@ -2793,7 +2781,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2819,7 +2807,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2845,7 +2833,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2871,7 +2859,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2897,7 +2885,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2923,7 +2911,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2</v>
       </c>
@@ -2949,7 +2937,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2</v>
       </c>
@@ -2975,7 +2963,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
@@ -3001,7 +2989,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4</v>
       </c>
@@ -3027,7 +3015,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>5</v>
       </c>
@@ -3053,7 +3041,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>6</v>
       </c>
@@ -3079,7 +3067,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>9</v>
       </c>
@@ -3105,7 +3093,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>9</v>
       </c>
@@ -3131,7 +3119,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>9</v>
       </c>
@@ -3157,7 +3145,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>9</v>
       </c>
@@ -3183,7 +3171,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>9</v>
       </c>
@@ -3209,7 +3197,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>10</v>
       </c>
@@ -3235,7 +3223,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>10</v>
       </c>
@@ -3261,7 +3249,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>11</v>
       </c>
@@ -3287,7 +3275,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>11</v>
       </c>
@@ -3313,7 +3301,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>12</v>
       </c>
@@ -3339,7 +3327,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>12</v>
       </c>
@@ -3365,7 +3353,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>22</v>
       </c>
@@ -3391,7 +3379,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>22</v>
       </c>
@@ -3425,7 +3413,7 @@
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1</v>
       </c>
@@ -3468,7 +3456,7 @@
       <c r="R44" s="3"/>
       <c r="S44" s="3"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1</v>
       </c>
@@ -3511,7 +3499,7 @@
       <c r="R45" s="3"/>
       <c r="S45" s="3"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1</v>
       </c>
@@ -3554,7 +3542,7 @@
       <c r="R46" s="3"/>
       <c r="S46" s="3"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2</v>
       </c>
@@ -3597,7 +3585,7 @@
       <c r="R47" s="3"/>
       <c r="S47" s="3"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1</v>
       </c>
@@ -3640,7 +3628,7 @@
       <c r="R48" s="3"/>
       <c r="S48" s="3"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>3</v>
       </c>
@@ -3683,7 +3671,7 @@
       <c r="R49" s="3"/>
       <c r="S49" s="3"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>8</v>
       </c>
@@ -3711,7 +3699,7 @@
       <c r="I50" s="3">
         <v>250000</v>
       </c>
-      <c r="J50" s="27">
+      <c r="J50" s="26">
         <v>50000000</v>
       </c>
       <c r="K50" s="3">
@@ -3734,7 +3722,7 @@
       <c r="R50" s="3"/>
       <c r="S50" s="3"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>8</v>
       </c>
@@ -3777,7 +3765,7 @@
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>8</v>
       </c>
@@ -3826,7 +3814,7 @@
       <c r="R52" s="3"/>
       <c r="S52" s="3"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>8</v>
       </c>
@@ -3869,7 +3857,7 @@
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>9</v>
       </c>
@@ -3920,7 +3908,7 @@
       <c r="R54" s="3"/>
       <c r="S54" s="3"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>9</v>
       </c>
@@ -3948,7 +3936,7 @@
       <c r="I55" s="3">
         <v>250000</v>
       </c>
-      <c r="J55" s="27">
+      <c r="J55" s="26">
         <v>50000000</v>
       </c>
       <c r="K55" s="3">
@@ -3962,7 +3950,7 @@
       <c r="R55" s="3"/>
       <c r="S55" s="3"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>10</v>
       </c>
@@ -3991,7 +3979,7 @@
         <v>650000</v>
       </c>
       <c r="J56" s="3">
-        <v>56500000000</v>
+        <v>117250000000</v>
       </c>
       <c r="K56" s="3">
         <v>17</v>
@@ -4004,7 +3992,7 @@
       <c r="R56" s="3"/>
       <c r="S56" s="3"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>11</v>
       </c>
@@ -4033,7 +4021,10 @@
         <v>0</v>
       </c>
       <c r="J57" s="3">
-        <v>0</v>
+        <v>117250000000</v>
+      </c>
+      <c r="K57" s="3">
+        <v>17</v>
       </c>
       <c r="L57" s="3"/>
       <c r="M57" s="21"/>
@@ -4044,7 +4035,7 @@
       <c r="R57" s="3"/>
       <c r="S57" s="3"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>11</v>
       </c>
@@ -4084,7 +4075,7 @@
       <c r="O58" s="17"/>
       <c r="P58" s="7"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>22</v>
       </c>
@@ -4121,7 +4112,7 @@
       <c r="O59" s="14"/>
       <c r="P59" s="3"/>
     </row>
-    <row r="60" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>22</v>
       </c>
@@ -4143,8 +4134,8 @@
       <c r="G60">
         <v>1</v>
       </c>
-      <c r="H60" s="26">
-        <v>0</v>
+      <c r="H60" s="24">
+        <v>2000000</v>
       </c>
       <c r="I60" s="3">
         <v>0</v>
@@ -4160,7 +4151,7 @@
       </c>
       <c r="P60" s="3"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="O62" t="s">
         <v>66</v>
       </c>
@@ -4175,19 +4166,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F55713-1448-49D9-BD60-FDB1E7BDCF91}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
@@ -4208,307 +4199,307 @@
       </c>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="27">
         <v>2023</v>
       </c>
-      <c r="D2" s="28">
+      <c r="D2" s="27">
         <v>150</v>
       </c>
-      <c r="E2" s="28">
+      <c r="E2" s="27">
         <v>110</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="27">
         <v>48550</v>
       </c>
       <c r="I2" s="17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="28" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="27">
         <v>2034</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="27">
         <v>150</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="27">
         <v>166</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="27">
         <v>25920</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="28" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="27">
         <v>2050</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="27">
         <v>150</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="27">
         <v>166</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="27">
         <v>25920</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="29" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="28">
         <v>2026</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="28">
         <v>150</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="29">
         <f>FORECAST($C5,E$2:E$4,$C$2:$C$4)</f>
         <v>128.7341772151899</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="29">
         <f>FORECAST($C5,F$2:F$4,$C$2:$C$4)</f>
         <v>40979.385171790142</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="29" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="28">
         <v>2028</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="28">
         <v>150</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="29">
         <f t="shared" ref="E6:F8" si="0">FORECAST($C6,E$2:E$4,$C$2:$C$4)</f>
         <v>132.58227848101251</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="29">
         <f t="shared" si="0"/>
         <v>39424.339963833569</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="29" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="28">
         <v>2030</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="28">
         <v>150</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="29">
         <f t="shared" si="0"/>
         <v>136.43037974683511</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="29">
         <f t="shared" si="0"/>
         <v>37869.294755876996</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="29" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="28">
         <v>2040</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="28">
         <v>150</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="29">
         <f t="shared" si="0"/>
         <v>155.67088607594906</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="29">
         <f t="shared" si="0"/>
         <v>30094.068716093898</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="28" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="27">
         <v>2023</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="27">
         <v>100</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="27">
         <v>10</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="27">
         <v>46430</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="28" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="27">
         <v>2034</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="27">
         <v>100</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="27">
         <v>20</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="27">
         <v>42000</v>
       </c>
       <c r="I10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="28" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="27">
         <v>2050</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="27">
         <v>100</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="27">
         <v>20</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="27">
         <v>37420</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="29" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="28">
         <v>2026</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="28">
         <v>100</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="29">
         <f>FORECAST($C12,E$9:E$11,$C$9:$C$11)</f>
         <v>13.345388788426703</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="29">
         <f>FORECAST($C12,F$9:F$11,$C$9:$C$11)</f>
         <v>45142.622061482864</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="29" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="28">
         <v>2028</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="28">
         <v>100</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="29">
         <f t="shared" ref="E13:F15" si="1">FORECAST($C13,E$9:E$11,$C$9:$C$11)</f>
         <v>14.032549728752201</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="29">
         <f t="shared" si="1"/>
         <v>44482.079566003638</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="29" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="28">
         <v>2030</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="28">
         <v>100</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="29">
         <f t="shared" si="1"/>
         <v>14.719710669077699</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="29">
         <f t="shared" si="1"/>
         <v>43821.537070524413</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="29" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="28">
         <v>2040</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="28">
         <v>100</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="29">
         <f t="shared" si="1"/>
         <v>18.155515370705189</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="29">
         <f t="shared" si="1"/>
         <v>40518.824593128404</v>
       </c>
@@ -4527,14 +4518,14 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>47</v>
       </c>
@@ -4542,74 +4533,58 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1d2ad661-40b4-4211-810e-9f8311f21e61" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085DB58C8134B304E8722528DF46508C9" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80174008b946241598c9c4dc1e838b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1d2ad661-40b4-4211-810e-9f8311f21e61" xmlns:ns4="e3bebc04-41cd-4c9b-8948-0bf19cce4780" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="83c7d99240e58c9b66f78776c092749e" ns3:_="" ns4:_="">
     <xsd:import namespace="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
@@ -4850,32 +4825,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1F09BEA-AF68-4060-8C78-FF3F1F123D80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="e3bebc04-41cd-4c9b-8948-0bf19cce4780"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153AE8AE-6581-44C9-9194-962A53477112}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1d2ad661-40b4-4211-810e-9f8311f21e61" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A60908BF-6965-4963-8A59-4F703B835956}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4892,4 +4859,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153AE8AE-6581-44C9-9194-962A53477112}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1F09BEA-AF68-4060-8C78-FF3F1F123D80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="e3bebc04-41cd-4c9b-8948-0bf19cce4780"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated fuel mix and nordnorgebanen cost
</commit_message>
<xml_diff>
--- a/Data/capacities_and_investments.xlsx
+++ b/Data/capacities_and_investments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonamar\Documents\04_Papers\Paper IV\Invest_capacity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruben\GitHub\STraM_ntnu_development\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFE2030-2E27-40C7-BB93-12FB8D99A0E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBE525C-3D91-4FCC-9100-8FA271B16203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="15996" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="node_capacities" sheetId="9" r:id="rId1"/>
@@ -20,6 +20,17 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataSignature="AMtx7mgsZk5PiUtOKDBIY/SuWxB5nEitHw=="/>
     </ext>
@@ -28,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="85">
   <si>
     <t>Oslo</t>
   </si>
@@ -277,6 +288,12 @@
   </si>
   <si>
     <t>the blue values are interpolated</t>
+  </si>
+  <si>
+    <t>We assign half of total cost of Nord-Norgebanen to our freight model (rest is a "passenger transport" investment)</t>
+  </si>
+  <si>
+    <t>From that, we assign half to each of the two stretches</t>
   </si>
 </sst>
 </file>
@@ -287,11 +304,18 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@"/>
     <numFmt numFmtId="165" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -422,6 +446,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -461,41 +491,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2239,8 +2271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF0D60D-EDFF-4BF0-A9C8-7E20F58C5774}">
   <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K57" sqref="K57"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2253,7 +2285,7 @@
     <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.109375" customWidth="1"/>
     <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
@@ -3979,14 +4011,17 @@
         <v>650000</v>
       </c>
       <c r="J56" s="3">
-        <v>117250000000</v>
+        <f>117250000000/2</f>
+        <v>58625000000</v>
       </c>
       <c r="K56" s="3">
         <v>17</v>
       </c>
       <c r="L56" s="3"/>
       <c r="N56" s="21"/>
-      <c r="O56" s="18"/>
+      <c r="O56" s="30" t="s">
+        <v>83</v>
+      </c>
       <c r="P56" s="3"/>
       <c r="Q56" s="3"/>
       <c r="R56" s="3"/>
@@ -4018,10 +4053,11 @@
         <v>0</v>
       </c>
       <c r="I57" s="3">
-        <v>0</v>
+        <v>650000</v>
       </c>
       <c r="J57" s="3">
-        <v>117250000000</v>
+        <f>117250000000/2</f>
+        <v>58625000000</v>
       </c>
       <c r="K57" s="3">
         <v>17</v>
@@ -4029,7 +4065,9 @@
       <c r="L57" s="3"/>
       <c r="M57" s="21"/>
       <c r="N57" s="21"/>
-      <c r="O57" s="18"/>
+      <c r="O57" s="31" t="s">
+        <v>84</v>
+      </c>
       <c r="P57" s="3"/>
       <c r="Q57" s="3"/>
       <c r="R57" s="3"/>
@@ -4585,6 +4623,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085DB58C8134B304E8722528DF46508C9" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80174008b946241598c9c4dc1e838b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1d2ad661-40b4-4211-810e-9f8311f21e61" xmlns:ns4="e3bebc04-41cd-4c9b-8948-0bf19cce4780" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="83c7d99240e58c9b66f78776c092749e" ns3:_="" ns4:_="">
     <xsd:import namespace="1d2ad661-40b4-4211-810e-9f8311f21e61"/>
@@ -4825,15 +4872,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4843,6 +4881,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153AE8AE-6581-44C9-9194-962A53477112}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A60908BF-6965-4963-8A59-4F703B835956}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4857,14 +4903,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153AE8AE-6581-44C9-9194-962A53477112}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>